<commit_message>
maj htp engagement 2
</commit_message>
<xml_diff>
--- a/engagementhtp.xlsx
+++ b/engagementhtp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9225" firstSheet="14" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="67">
   <si>
     <t>Ligne</t>
   </si>
@@ -74,12 +74,6 @@
     <t>/23h/</t>
   </si>
   <si>
-    <t>\17h\</t>
-  </si>
-  <si>
-    <t>\23h\</t>
-  </si>
-  <si>
     <t>htpfacmg16</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
     <t>/RETOUR_MGEFI_GTO/Noemie/</t>
   </si>
   <si>
-    <t>\RETOUR_MGEFI_GTO\Noemie\</t>
-  </si>
-  <si>
     <t>FENENR</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
     <t>htpfluxfin</t>
   </si>
   <si>
-    <t>\RETOUR_MGEFI_GTO\rejet def\</t>
-  </si>
-  <si>
     <t>/RETOUR_MGEFI_GTO/rejet def/</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>MGEFI_Rejets_saisies_noemie_HTP</t>
   </si>
   <si>
-    <t>\RETOUR_ADHESION_LAMIE\</t>
-  </si>
-  <si>
     <t>/RETOUR_ADHESION_LAMIE/</t>
   </si>
   <si>
@@ -158,18 +143,12 @@
     <t>/RETOUR_ADHESION_CSS/adhesion ITE/</t>
   </si>
   <si>
-    <t>\RETOUR_ADHESION_CSS\adhesion ITE\</t>
-  </si>
-  <si>
     <t>Suivi Saisie Prod ITE</t>
   </si>
   <si>
     <t>/RETOUR_ADHESION_CSS/adhesion MGAS/</t>
   </si>
   <si>
-    <t>\RETOUR_ADHESION_CSS\adhesion MGAS\</t>
-  </si>
-  <si>
     <t>Suivi Saisie Prod MGAS</t>
   </si>
   <si>
@@ -185,9 +164,6 @@
     <t>/RETOUR_ADHESION_CSS/adhesion LMDE/</t>
   </si>
   <si>
-    <t>\RETOUR_ADHESION_CSS\adhesion LMDE\</t>
-  </si>
-  <si>
     <t>Saisie Prod LMDE</t>
   </si>
   <si>
@@ -218,9 +194,6 @@
     <t>/SALESFORCE/</t>
   </si>
   <si>
-    <t>\SALESFORCE\</t>
-  </si>
-  <si>
     <t>TRAME SALESFORCE</t>
   </si>
   <si>
@@ -251,9 +224,6 @@
     <t>/</t>
   </si>
   <si>
-    <t>\</t>
-  </si>
-  <si>
     <t>htpfacmgtnontj</t>
   </si>
   <si>
@@ -276,9 +246,6 @@
   </si>
   <si>
     <t>htpdevitnontj5</t>
-  </si>
-  <si>
-    <t>23h</t>
   </si>
 </sst>
 </file>
@@ -633,8 +600,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
@@ -862,7 +829,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,13 +839,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -887,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -896,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -915,7 +882,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,13 +893,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -941,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -950,21 +917,21 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -973,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -982,10 +949,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +968,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1010,13 +979,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1025,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1034,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1053,27 +1022,27 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
@@ -1081,10 +1050,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1100,17 +1069,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1119,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1128,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1147,17 +1116,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1166,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1175,10 +1144,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1194,17 +1163,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1213,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1222,10 +1191,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1241,17 +1210,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1260,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1269,10 +1238,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1288,17 +1257,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1307,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1316,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1335,17 +1304,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1354,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1363,10 +1332,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1383,7 +1352,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1365,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1408,19 +1377,19 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -1428,7 +1397,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1440,19 +1409,19 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
@@ -1473,17 +1442,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1492,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1501,10 +1470,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1520,17 +1489,17 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1539,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1548,10 +1517,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1566,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,10 +1546,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -1589,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1598,10 +1567,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1618,7 +1587,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1598,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1641,19 +1610,19 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -1661,7 +1630,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1673,19 +1642,19 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
         <v>3</v>
@@ -1705,7 +1674,9 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1719,23 +1690,23 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
@@ -1743,22 +1714,22 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
@@ -1766,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -1775,85 +1746,85 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
         <v>25</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1862,7 +1833,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -1871,21 +1842,21 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1894,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -1903,31 +1874,31 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
@@ -1935,21 +1906,21 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1958,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
         <v>0</v>
@@ -1967,21 +1938,21 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1990,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
@@ -1999,21 +1970,21 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2022,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
         <v>0</v>
@@ -2031,21 +2002,21 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2054,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
         <v>0</v>
@@ -2063,21 +2034,21 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2086,7 +2057,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
         <v>0</v>
@@ -2095,10 +2066,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2124,14 +2095,14 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -2143,19 +2114,19 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -2177,14 +2148,14 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -2196,19 +2167,19 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -2230,14 +2201,14 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -2249,19 +2220,19 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -2280,14 +2251,14 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -2299,19 +2270,19 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -2330,7 +2301,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2341,13 +2312,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -2356,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -2365,10 +2336,10 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj chemin htp engagement
</commit_message>
<xml_diff>
--- a/engagementhtp.xlsx
+++ b/engagementhtp.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="69">
   <si>
     <t>Ligne</t>
   </si>
@@ -248,7 +248,10 @@
     <t>htpdevitnontj5</t>
   </si>
   <si>
-    <t>SALESFORCE/</t>
+    <t>SALESFORCE</t>
+  </si>
+  <si>
+    <t>SALESFORCE\</t>
   </si>
 </sst>
 </file>
@@ -885,7 +888,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
mise a jour bouton engagement htp
</commit_message>
<xml_diff>
--- a/engagementhtp.xlsx
+++ b/engagementhtp.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil11" sheetId="11" r:id="rId3"/>
+    <sheet name="Feuil3" sheetId="11" r:id="rId3"/>
     <sheet name="Feuil12" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="69">
   <si>
     <t>Ligne</t>
   </si>
@@ -588,7 +588,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1834,15 +1834,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="86.7109375" customWidth="1"/>
+    <col min="1" max="1" width="99.140625" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
@@ -1912,10 +1912,43 @@
         <v>49</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="\\10.128.1.2\bpo_almerys\"/>
     <hyperlink ref="A2" r:id="rId2" display="\\10.128.1.2\bpo_almerys\"/>
+    <hyperlink ref="A3" r:id="rId3" display="\\10.128.1.2\bpo_almerys\"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1926,13 +1959,15 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
maj export htp engagement
</commit_message>
<xml_diff>
--- a/engagementhtp.xlsx
+++ b/engagementhtp.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="69">
   <si>
     <t>Ligne</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>/RETOUR_ADHESION_LAMIE/</t>
-  </si>
-  <si>
-    <t>Trame_LAMIE_Stocks_V2</t>
   </si>
   <si>
     <t>Nom du fichier</t>
@@ -672,7 +669,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -704,7 +701,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -736,7 +733,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -768,7 +765,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -800,7 +797,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -815,7 +812,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>13</v>
@@ -832,7 +829,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
@@ -847,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>13</v>
@@ -864,7 +861,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -879,7 +876,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>13</v>
@@ -896,7 +893,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -911,7 +908,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>13</v>
@@ -928,10 +925,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
@@ -941,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>0</v>
@@ -950,18 +947,18 @@
         <v>0</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
@@ -971,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>0</v>
@@ -980,18 +977,18 @@
         <v>0</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
@@ -1001,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>0</v>
@@ -1010,18 +1007,18 @@
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
@@ -1031,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>0</v>
@@ -1040,18 +1037,18 @@
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
@@ -1061,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>0</v>
@@ -1070,18 +1067,18 @@
         <v>0</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
@@ -1091,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>0</v>
@@ -1100,18 +1097,18 @@
         <v>0</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
@@ -1121,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>0</v>
@@ -1130,18 +1127,18 @@
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
@@ -1151,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>0</v>
@@ -1160,18 +1157,18 @@
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
@@ -1181,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>0</v>
@@ -1190,18 +1187,18 @@
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3">
@@ -1211,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>0</v>
@@ -1220,10 +1217,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1353,7 +1350,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,16 +1499,16 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -1523,7 +1520,7 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1534,7 +1531,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1543,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -1555,7 +1552,7 @@
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1563,31 +1560,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1595,31 +1592,31 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1627,31 +1624,31 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1659,31 +1656,31 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1691,31 +1688,31 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1723,31 +1720,31 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1758,7 +1755,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1767,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
@@ -1779,7 +1776,7 @@
         <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1790,7 +1787,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1799,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
@@ -1811,7 +1808,7 @@
         <v>26</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1853,98 +1850,98 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="J2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="J3" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1975,34 +1972,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj export stock htp engagement
</commit_message>
<xml_diff>
--- a/engagementhtp.xlsx
+++ b/engagementhtp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9225"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="68">
   <si>
     <t>Ligne</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>//10.128.1.2/bpo_almerys/00-TOUS/06-DOSSIER POLE/01-HTTP/05- REPORTING/03-HTP/DOC_HTP</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>htpfacmgtnontj</t>
@@ -588,8 +585,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +925,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
@@ -947,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>53</v>
@@ -958,7 +955,7 @@
         <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3">
@@ -977,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>53</v>
@@ -988,7 +985,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
@@ -998,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>0</v>
@@ -1007,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>53</v>
@@ -1018,7 +1015,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
@@ -1028,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>0</v>
@@ -1037,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>53</v>
@@ -1048,7 +1045,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
@@ -1058,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>0</v>
@@ -1067,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>53</v>
@@ -1078,7 +1075,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
@@ -1088,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>0</v>
@@ -1097,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>53</v>
@@ -1108,7 +1105,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
@@ -1118,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>0</v>
@@ -1127,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>53</v>
@@ -1138,7 +1135,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
@@ -1148,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>0</v>
@@ -1157,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>53</v>
@@ -1168,7 +1165,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
@@ -1178,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>0</v>
@@ -1187,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>53</v>
@@ -1198,7 +1195,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3">
@@ -1208,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>0</v>
@@ -1217,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>53</v>
@@ -1349,8 +1346,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1517,7 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1552,7 +1549,7 @@
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1776,7 +1773,7 @@
         <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1808,7 +1805,7 @@
         <v>26</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1850,7 +1847,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
@@ -1874,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
         <v>48</v>
@@ -1882,7 +1879,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -1906,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
         <v>48</v>
@@ -1914,7 +1911,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
@@ -1938,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
         <v>48</v>

</xml_diff>